<commit_message>
Update code handle for many bill
</commit_message>
<xml_diff>
--- a/list_invoice.xlsx
+++ b/list_invoice.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/b/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/b/Works/MyProject/pdf-compare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DC54B3-D9F1-344A-AADF-CCAD3207D583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EA32B2-553C-AD43-A8CB-F8F8AAD7F011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16860" xr2:uid="{B6D6C27F-2619-465E-AF87-A24221B0FECE}"/>
   </bookViews>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
-  <si>
-    <t>ac6e9642-a891-426e-ba2f-c1d21b4decf0/5ec140dc-a169-11ef-927e-42010ac1e0d9/Jaarafrekening_F0483115</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
   <si>
     <t>d2942f13-fa4d-4b62-a36e-1223cf6bc34c/e3ae16ba-0b46-11ef-8a2b-42010ac1e0cd/Eindafrekening_F0300358</t>
   </si>
@@ -49,13 +46,244 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>68d3ed71-90d0-4233-97b8-51ca8d0cff0c/b6fefc01-4cbf-11f0-ac29-42010ac1e211/Jaarafrekening_F0669372</t>
+  </si>
+  <si>
+    <t>68d3ed71-90d0-4233-97b8-51ca8d0cff0c/c6544710-d02b-11ef-8afd-42010ac1e0d9/Jaarafrekening_F0530520</t>
+  </si>
+  <si>
+    <t>8563aad0-e524-4842-a159-4242b46fb812/da13698b-c7db-11ef-8afd-42010ac1e0d9/Eindafrekening_F0522197</t>
+  </si>
+  <si>
+    <t>8563aad0-e524-4842-a159-4242b46fb812/da13698b-c7db-11ef-8afd-42010ac1e0d9/Eindafrekening_F0669382</t>
+  </si>
+  <si>
+    <t>ac6e9642-a891-426e-ba2f-c1d21b4decf0/5447cdef-cafe-11ef-8afd-42010ac1e0d9/Eindafrekening_F0528792</t>
+  </si>
+  <si>
+    <t>ac6e9642-a891-426e-ba2f-c1d21b4decf0/5447cdef-cafe-11ef-8afd-42010ac1e0d9/Eindafrekening_F0669383</t>
+  </si>
+  <si>
+    <t>68d3ed71-90d0-4233-97b8-51ca8d0cff0c/c6544710-d02b-11ef-8afd-42010ac1e0d9/Jaarafrekening_F0669372</t>
+  </si>
+  <si>
+    <t>ac6e9642-a891-426e-ba2f-c1d21b4decf0/5bcc17e5-d2ae-11ef-bd30-42010ac1e0de/Eindafrekening_F0504522</t>
+  </si>
+  <si>
+    <t>ac6e9642-a891-426e-ba2f-c1d21b4decf0/5bcc17e5-d2ae-11ef-bd30-42010ac1e0de/Eindafrekening_F0669381</t>
+  </si>
+  <si>
+    <t>c28eedab-b42d-47ec-8433-f441c0092df2/332c0014-d8b5-11ef-bd30-42010ac1e0de/Eindafrekening_F0543665</t>
+  </si>
+  <si>
+    <t>c28eedab-b42d-47ec-8433-f441c0092df2/332c0014-d8b5-11ef-bd30-42010ac1e0de/Eindafrekening_F0669375</t>
+  </si>
+  <si>
+    <t>7804b423-c0d9-44e9-8fce-16a956faa75a/b46b53db-d9ee-11ef-bd30-42010ac1e0de/Eindafrekening_F0543843</t>
+  </si>
+  <si>
+    <t>7804b423-c0d9-44e9-8fce-16a956faa75a/b46b53db-d9ee-11ef-bd30-42010ac1e0de/Eindafrekening_F0669376</t>
+  </si>
+  <si>
+    <t>a6cbd610-f533-4947-a51d-1eb5fae908a0/4383c513-dd57-11ef-bd30-42010ac1e0de/Eindafrekening_F0545018</t>
+  </si>
+  <si>
+    <t>a6cbd610-f533-4947-a51d-1eb5fae908a0/4383c513-dd57-11ef-bd30-42010ac1e0de/Eindafrekening_F0669373</t>
+  </si>
+  <si>
+    <t>5f2d0f8e-ad74-4c6c-8d06-59907bf2c509/6406baaf-de73-11ef-bd30-42010ac1e0de/Jaarafrekening_F0545863</t>
+  </si>
+  <si>
+    <t>5f2d0f8e-ad74-4c6c-8d06-59907bf2c509/6406baaf-de73-11ef-bd30-42010ac1e0de/Jaarafrekening_F0669374</t>
+  </si>
+  <si>
+    <t>bcf5bb40-88c1-4629-b12e-bab23a8116d8/fda696b7-de81-11ef-bd30-42010ac1e0de/Jaarafrekening_F0545893</t>
+  </si>
+  <si>
+    <t>bcf5bb40-88c1-4629-b12e-bab23a8116d8/fda696b7-de81-11ef-bd30-42010ac1e0de/Jaarafrekening_F0669377</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/ed6a4e59-e11f-11ef-bd30-42010ac1e0de/Eindafrekening_F0552148</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/ed6a4e59-e11f-11ef-bd30-42010ac1e0de/Eindafrekening_F0669388</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/276ab7e9-e1cc-11ef-bd30-42010ac1e0de/Eindafrekening_F0552222</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/276ab7e9-e1cc-11ef-bd30-42010ac1e0de/Eindafrekening_F0669386</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/e0a37012-e1d0-11ef-bd30-42010ac1e0de/Eindafrekening_F0552226</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/e0a37012-e1d0-11ef-bd30-42010ac1e0de/Eindafrekening_F0669604</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/1c9538ad-e1f0-11ef-bd30-42010ac1e0de/Eindafrekening_F0552712</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/1c9538ad-e1f0-11ef-bd30-42010ac1e0de/Eindafrekening_F0669605</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/b1dda0d0-e23d-11ef-bd30-42010ac1e0de/Eindafrekening_F0552782</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/b1dda0d0-e23d-11ef-bd30-42010ac1e0de/Eindafrekening_F0669606</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/1dd2f08b-e314-11ef-bd30-42010ac1e0de/Eindafrekening_F0553194</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/1dd2f08b-e314-11ef-bd30-42010ac1e0de/Eindafrekening_F0669607</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/ccf7e34e-e314-11ef-bd30-42010ac1e0de/Eindafrekening_F0553198</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/ccf7e34e-e314-11ef-bd30-42010ac1e0de/Eindafrekening_F0669608</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/5289f23e-e326-11ef-bd30-42010ac1e0de/Eindafrekening_F0553220</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/5289f23e-e326-11ef-bd30-42010ac1e0de/Eindafrekening_F0669609</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/adcddede-e32f-11ef-bd30-42010ac1e0de/Eindafrekening_F0553233</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/adcddede-e32f-11ef-bd30-42010ac1e0de/Eindafrekening_F0669610</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/02545b0d-e88a-11ef-bd30-42010ac1e0de/Eindafrekening_F0555103</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/02545b0d-e88a-11ef-bd30-42010ac1e0de/Eindafrekening_F0669611</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/930e93fe-e894-11ef-bd30-42010ac1e0de/Eindafrekening_F0555115</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/930e93fe-e894-11ef-bd30-42010ac1e0de/Eindafrekening_F0669612</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/88b46ace-e8bb-11ef-bd30-42010ac1e0de/Eindafrekening_F0555159</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/88b46ace-e8bb-11ef-bd30-42010ac1e0de/Eindafrekening_F0669614</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/84c42087-e955-11ef-bd30-42010ac1e0de/Eindafrekening_F0555440</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/84c42087-e955-11ef-bd30-42010ac1e0de/Eindafrekening_F0669387</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/b9377ac0-ea46-11ef-bd30-42010ac1e0de/Eindafrekening_F0564794</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/b9377ac0-ea46-11ef-bd30-42010ac1e0de/Eindafrekening_F0669615</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/bd4c55df-ee14-11ef-bd30-42010ac1e0de/Eindafrekening_F0567296</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/bd4c55df-ee14-11ef-bd30-42010ac1e0de/Eindafrekening_F0669616</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/72076d64-f543-11ef-bd30-42010ac1e0de/Eindafrekening_F0569453</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/72076d64-f543-11ef-bd30-42010ac1e0de/Eindafrekening_F0669617</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/d36ee436-f543-11ef-bd30-42010ac1e0de/Eindafrekening_F0569454</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/d36ee436-f543-11ef-bd30-42010ac1e0de/Eindafrekening_F0669618</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/1aae5ec1-f54c-11ef-bd30-42010ac1e0de/Eindafrekening_F0569466</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/1aae5ec1-f54c-11ef-bd30-42010ac1e0de/Eindafrekening_F0669619</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/8e13b8bc-f91a-11ef-bd30-42010ac1e0de/Eindafrekening_F0576408</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/8e13b8bc-f91a-11ef-bd30-42010ac1e0de/Eindafrekening_F0669620</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/103a74bf-00a2-11f0-92ce-42010ac1e209/Eindafrekening_F0588064</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/103a74bf-00a2-11f0-92ce-42010ac1e209/Eindafrekening_F0669621</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/5c185492-00a2-11f0-92ce-42010ac1e209/Eindafrekening_F0588065</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/5c185492-00a2-11f0-92ce-42010ac1e209/Eindafrekening_F0669622</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/b6477e4d-00aa-11f0-92ce-42010ac1e209/Eindafrekening_F0588102</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/b6477e4d-00aa-11f0-92ce-42010ac1e209/Eindafrekening_F0669623</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/a550ab19-02e2-11f0-92ce-42010ac1e209/Eindafrekening_F0589885</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/a550ab19-02e2-11f0-92ce-42010ac1e209/Eindafrekening_F0669624</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/fa10bfe5-02e5-11f0-92ce-42010ac1e209/Eindafrekening_F0590140</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/fa10bfe5-02e5-11f0-92ce-42010ac1e209/Eindafrekening_F0669625</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/3e25ec81-02f0-11f0-92ce-42010ac1e209/Eindafrekening_F0590167</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/3e25ec81-02f0-11f0-92ce-42010ac1e209/Eindafrekening_F0669626</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/ae3ae53f-0b14-11f0-92ce-42010ac1e209/Eindafrekening_F0592602</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/ae3ae53f-0b14-11f0-92ce-42010ac1e209/Eindafrekening_F0669627</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/f1e0837f-1c41-11f0-92ce-42010ac1e209/Eindafrekening_F0613330</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/f1e0837f-1c41-11f0-92ce-42010ac1e209/Eindafrekening_F0669628</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/a018ffe5-1c47-11f0-92ce-42010ac1e209/Eindafrekening_F0613355</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/a018ffe5-1c47-11f0-92ce-42010ac1e209/Eindafrekening_F0669629</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/c55e83a3-1eb0-11f0-92ce-42010ac1e209/Eindafrekening_F0614194</t>
+  </si>
+  <si>
+    <t>e3af665d-b88e-4402-9b81-dfda0e04ff7f/c55e83a3-1eb0-11f0-92ce-42010ac1e209/Eindafrekening_F0669630</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +340,12 @@
       <color rgb="FF4EA72E"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -171,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -194,6 +428,7 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,7 +766,7 @@
   <dimension ref="A1:B1347"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -541,171 +776,323 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
+      <c r="B2" s="22" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="A25" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="A27" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="A28" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
+      <c r="A30" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="A31" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
+      <c r="A32" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+      <c r="A33" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="A34" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+      <c r="A35" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="1"/>
+      <c r="A36" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+      <c r="A37" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+      <c r="A38" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
+      <c r="A39" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
+      <c r="A40" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
@@ -5948,7 +6335,7 @@
   <dimension ref="A1:B392"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" activeCellId="1" sqref="A5 A16"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5958,10 +6345,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>